<commit_message>
Reparación de bug y pruebas de unidad
Se econtró un bug en el CU de Editar cliente el cual fue corregido y se realizaron las pruebas unitarias correspondientes a los métodos implementados anteriormente
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 6/Plantilla de Casos de Uso .xlsx
+++ b/Plantillas/Entrega 6/Plantilla de Casos de Uso .xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B67BC7-8BF7-4CB2-9E32-A95FD4B58B8E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E2C345-803D-4001-955C-1A671A785879}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,9 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -967,7 +965,7 @@
         <v>5.44</v>
       </c>
       <c r="G5" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>65</v>
@@ -991,7 +989,7 @@
         <v>0.66</v>
       </c>
       <c r="G6" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>65</v>
@@ -1015,7 +1013,7 @@
         <v>0.22</v>
       </c>
       <c r="G7" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>65</v>
@@ -1039,7 +1037,7 @@
         <v>0.37</v>
       </c>
       <c r="G8" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>65</v>
@@ -1057,13 +1055,13 @@
         <v>51</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F9" s="11">
         <v>14.16</v>
       </c>
       <c r="G9" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>65</v>
@@ -1083,13 +1081,13 @@
         <v>52</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F10" s="11">
         <v>13.75</v>
       </c>
       <c r="G10" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>65</v>
@@ -1109,13 +1107,13 @@
         <v>53</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F11" s="11">
         <v>13.26</v>
       </c>
       <c r="G11" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>65</v>
@@ -1135,13 +1133,13 @@
         <v>54</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F12" s="11">
         <v>16.29</v>
       </c>
       <c r="G12" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>65</v>
@@ -1167,7 +1165,7 @@
         <v>0.41</v>
       </c>
       <c r="G13" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>65</v>
@@ -1191,7 +1189,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>65</v>
@@ -1215,7 +1213,7 @@
         <v>24.33</v>
       </c>
       <c r="G15" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>65</v>
@@ -1239,7 +1237,7 @@
         <v>15.58</v>
       </c>
       <c r="G16" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>65</v>
@@ -1263,7 +1261,7 @@
         <v>23.5</v>
       </c>
       <c r="G17" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>65</v>
@@ -1287,7 +1285,7 @@
         <v>16.559999999999999</v>
       </c>
       <c r="G18" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>65</v>
@@ -1311,7 +1309,7 @@
         <v>6.82</v>
       </c>
       <c r="G19" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="6"/>
@@ -1333,7 +1331,7 @@
         <v>11.75</v>
       </c>
       <c r="G20" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>65</v>
@@ -1357,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>65</v>
@@ -1381,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>65</v>
@@ -1405,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>65</v>
@@ -1429,7 +1427,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G24" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>65</v>
@@ -1453,7 +1451,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="G25" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>65</v>
@@ -1477,7 +1475,7 @@
         <v>0.16</v>
       </c>
       <c r="G26" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>65</v>
@@ -1501,7 +1499,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="G27" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>65</v>
@@ -1525,7 +1523,7 @@
         <v>0.26</v>
       </c>
       <c r="G28" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>65</v>
@@ -1549,7 +1547,7 @@
         <v>0.66</v>
       </c>
       <c r="G29" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>65</v>
@@ -1573,7 +1571,7 @@
         <v>10.63</v>
       </c>
       <c r="G30" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>65</v>
@@ -1597,7 +1595,7 @@
         <v>3.35</v>
       </c>
       <c r="G31" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>65</v>
@@ -1621,7 +1619,7 @@
         <v>4.53</v>
       </c>
       <c r="G32" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>65</v>
@@ -1639,13 +1637,13 @@
         <v>75</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F33" s="11">
         <v>4.7699999999999996</v>
       </c>
       <c r="G33" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>65</v>
@@ -1663,11 +1661,13 @@
         <v>112</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="21"/>
+        <v>118</v>
+      </c>
+      <c r="F34" s="21">
+        <v>5</v>
+      </c>
       <c r="G34" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>65</v>
@@ -1685,11 +1685,13 @@
         <v>111</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="21"/>
+        <v>118</v>
+      </c>
+      <c r="F35" s="21">
+        <v>4.5</v>
+      </c>
       <c r="G35" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>65</v>
@@ -1711,7 +1713,7 @@
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="20">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>65</v>
@@ -1743,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B8" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Avance para sexta entrega
Se realizaron avances para la sexta entrega, incluyendo en su mayoria diagramas de robustez, de secuencia e interfaces graficas. También se añadió un caso de uso quitandole funcionalidades a otros casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 6/Plantilla de Casos de Uso .xlsx
+++ b/Plantillas/Entrega 6/Plantilla de Casos de Uso .xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E2C345-803D-4001-955C-1A671A785879}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3960DB-6A40-4099-8F48-719247BE47F2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,7 +894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1034,7 +1036,7 @@
         <v>105</v>
       </c>
       <c r="F8" s="11">
-        <v>0.37</v>
+        <v>3.37</v>
       </c>
       <c r="G8" s="20">
         <v>0.9</v>
@@ -1424,7 +1426,7 @@
         <v>105</v>
       </c>
       <c r="F24" s="11">
-        <v>0.57999999999999996</v>
+        <v>5.58</v>
       </c>
       <c r="G24" s="20">
         <v>0.9</v>
@@ -1472,7 +1474,7 @@
         <v>105</v>
       </c>
       <c r="F26" s="11">
-        <v>0.16</v>
+        <v>6.16</v>
       </c>
       <c r="G26" s="20">
         <v>0.9</v>
@@ -1520,7 +1522,7 @@
         <v>105</v>
       </c>
       <c r="F28" s="11">
-        <v>0.26</v>
+        <v>5.76</v>
       </c>
       <c r="G28" s="20">
         <v>0.9</v>
@@ -1568,7 +1570,7 @@
         <v>105</v>
       </c>
       <c r="F30" s="11">
-        <v>10.63</v>
+        <v>15.63</v>
       </c>
       <c r="G30" s="20">
         <v>0.9</v>
@@ -1616,7 +1618,7 @@
         <v>105</v>
       </c>
       <c r="F32" s="21">
-        <v>4.53</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="G32" s="20">
         <v>0.9</v>
@@ -1711,7 +1713,9 @@
       <c r="E36" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11">
+        <v>10</v>
+      </c>
       <c r="G36" s="20">
         <v>0.9</v>
       </c>

</xml_diff>